<commit_message>
Added 4 video tutorials on Git and Github
</commit_message>
<xml_diff>
--- a/video tutorials.xlsx
+++ b/video tutorials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\111ar\Desktop\Github repo\CodingEasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746F02E-D8A6-4DC7-ACBB-DA2C95D1F145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{7746F02E-D8A6-4DC7-ACBB-DA2C95D1F145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A1785CF-7429-4B4C-B6AB-986FF0D9F8FC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="4" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,39 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>GD link</t>
+  </si>
+  <si>
+    <t>Youtube link</t>
+  </si>
   <si>
     <t>C++</t>
   </si>
@@ -37,29 +59,44 @@
     <t>Git Github</t>
   </si>
   <si>
-    <t>HTML</t>
+    <t>Utkarsh Rai</t>
+  </si>
+  <si>
+    <t>Introduction to Git &amp; Github</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1OzNETc6oe5tDewQivYgt0elq6NfQ0BRz/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git status command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RRFCBk8WkjKQj91gcCRLCrFmAXOpLVo0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git add command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1yBP7n8PpCNyAX4891f0uQ8FIk9brSEDg/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git init command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1NuG7XGedxh919clWwoaQYo33TTC0WhZ_/view</t>
   </si>
   <si>
     <t>Python</t>
   </si>
   <si>
     <t>CSS</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>GD link</t>
-  </si>
-  <si>
-    <t>Youtube link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +128,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,16 +173,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,28 +472,28 @@
       <selection activeCell="G3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:8" ht="30.95">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -448,24 +511,24 @@
       <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -476,34 +539,81 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07166FE-884A-4003-9E51-9A65DF02B245}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="82.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{B2A65F9B-BACA-4DCA-B89D-01F078FD5072}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{4039BF5F-27CC-4DAA-B4F4-2C7BE2B695BA}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{8C703322-1A4A-4C9A-8753-F84F5D9EE460}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{FD706B4F-429A-4600-BDF2-B6C79EC23D91}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -516,24 +626,24 @@
       <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -546,28 +656,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28238582-452B-4AD2-8C73-8CBEF50BECA9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added video tutorials on topic: Git and Github (Length is more than 5 min. for both)
</commit_message>
<xml_diff>
--- a/video tutorials.xlsx
+++ b/video tutorials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\111ar\Desktop\Github repo\CodingEasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE842877-A23C-4F7A-802C-C37D0A1A881A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{7746F02E-D8A6-4DC7-ACBB-DA2C95D1F145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F70A8D2-E9A6-4DA8-94D0-5F57D7AC2186}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>HTML</t>
   </si>
@@ -83,44 +86,32 @@
     <t>https://drive.google.com/file/d/1NuG7XGedxh919clWwoaQYo33TTC0WhZ_/view</t>
   </si>
   <si>
+    <t>Pull Request 2 :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git checkout command </t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1_5D4bIORFzLN18LDjj7bO9uhF9TFJ8_6/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>git commit command</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Q_wcBNGOJTEXDwXPye8OW8TXdkjtzEY0/view?usp=sharing</t>
+  </si>
+  <si>
     <t>Python</t>
   </si>
   <si>
     <t>CSS</t>
-  </si>
-  <si>
-    <t>Vaibhav Srivastava</t>
-  </si>
-  <si>
-    <t>introduction and inline css</t>
-  </si>
-  <si>
-    <t>internal css</t>
-  </si>
-  <si>
-    <t>external css</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1S02OH6EZjlzxz9KfOIrDWDhgS_llVmp9/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1SrCXuA_XMPLTHRrBVq6RPEn8OOwghX7s/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1gyQwiPl36IPhVjEgy71GCeE8IrrXE0NI/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>css and its syntax</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1oxg3c5C1gSuk_7QC-GgRYxK4bYJ7_Xo8/view?usp=sharing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -201,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -209,6 +206,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -496,18 +494,18 @@
       <selection activeCell="G3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:8" ht="30.95">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,14 +533,14 @@
       <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -563,29 +561,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07166FE-884A-4003-9E51-9A65DF02B245}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="3" max="3" width="82.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -599,7 +597,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -607,7 +605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -615,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -623,13 +621,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="C14" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -637,6 +662,8 @@
     <hyperlink ref="C6" r:id="rId2" xr:uid="{4039BF5F-27CC-4DAA-B4F4-2C7BE2B695BA}"/>
     <hyperlink ref="C7" r:id="rId3" xr:uid="{8C703322-1A4A-4C9A-8753-F84F5D9EE460}"/>
     <hyperlink ref="C8" r:id="rId4" xr:uid="{FD706B4F-429A-4600-BDF2-B6C79EC23D91}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{AD636177-F169-4B57-8D35-E436C9A25A64}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{336EE910-2C81-4BE1-A76D-C648DE397C71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -650,14 +677,14 @@
       <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -678,23 +705,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28238582-452B-4AD2-8C73-8CBEF50BECA9}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -708,45 +732,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{E48C8BA2-4548-4594-A079-009F75343684}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{2B75073C-1282-4296-A6E7-D328659C18BA}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{91164D0A-37C0-4FF8-8FB5-BAFAE36260D1}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{E8AD5276-C9F5-483D-9C73-6115A171EACA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>